<commit_message>
FrontEnd And Backend Ready Of Manifest Data for Deployment
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-manifest-data.xlsx
+++ b/src/main/resources/excel-manifest-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stepway\smsa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AB9CFAA-C1C4-410D-9307-9FEAFD1F8852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D82FC3-B4B1-4452-A67D-D04D453CF448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Account Number</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Shipment Code</t>
+  </si>
+  <si>
+    <t>Consignee Name</t>
+  </si>
+  <si>
+    <t>Consignee City</t>
   </si>
 </sst>
 </file>
@@ -433,11 +439,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +475,7 @@
     <col min="25" max="16384" width="12.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -541,6 +547,12 @@
       </c>
       <c r="X1" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>